<commit_message>
finished table and test methods
</commit_message>
<xml_diff>
--- a/AUC.xlsx
+++ b/AUC.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Google Drive\Faculdade\Verificação e Validação de Software\Assignment1\vvs1920_assignment1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7835C79F-C602-4F8E-AECE-CA9AF2B45B23}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFADDC4A-5F3C-4D96-81E2-5BC10EF7BD90}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E18B8583-D319-4337-B06E-00832F8818CE}"/>
+    <workbookView xWindow="-7455" yWindow="5910" windowWidth="15375" windowHeight="7965" xr2:uid="{E18B8583-D319-4337-B06E-00832F8818CE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="112">
   <si>
     <t>query</t>
   </si>
@@ -146,44 +146,1550 @@
     <t>du(node,var)</t>
   </si>
   <si>
-    <t>[1,2], [1,3], [1,3,4], [1,3,5], [1,3,5,6,7], [1,3,5,6,8]</t>
-  </si>
-  <si>
     <t>[5,6,7]</t>
   </si>
   <si>
     <t>[13,14,6,7]</t>
   </si>
   <si>
-    <t>[5,6,7], [5,6,8], [5,6,8,10], [5,6,8,9], [5,6,8,9,11], [5,6,8,9,12], [5,6,8,9,12.13], [5,6,8,9,12,14]</t>
-  </si>
-  <si>
-    <t>[11,6,7], [11,6,8], [11,6,8,10], [11,6,8,9], [11,6,8,9,11], [11,6,8,9,12], [11,6,8,9,12.13], [11,6,8,9,12,14]</t>
-  </si>
-  <si>
-    <t>[10,6,7], [10,6,8], [10,6,8,10], [10,6,8,9], [10,6,8,9,11], [10,6,8,9,12], [10,6,8,9,12.13], [10,6,8,9,12,14]</t>
-  </si>
-  <si>
-    <t>[14,6,7], [14,6,8], [14,6,8,10], [14,6,8,9], [14,6,8,9,11], [14,6,8,9,12], [14,6,8,9,12.13], [14,6,8,9,12,14]</t>
-  </si>
-  <si>
-    <t>[5,6,7], [5,6,8], [5,6,9,12], [5,6,9,12,13]</t>
-  </si>
-  <si>
-    <t>[12,13], [12,13,14,6,7], [12,13,14,6,8], [12,13,14,6,8,9,12], [12,14,6,7], [12,14,6,8], [12,14,6,8,9,12]</t>
-  </si>
-  <si>
-    <t>[8,9], [8,10], [8,9,11], [8,9,12]</t>
+    <t>{root, query}</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>(input, expected)</t>
+  </si>
+  <si>
+    <t>test path</t>
+  </si>
+  <si>
+    <t>t1</t>
+  </si>
+  <si>
+    <t>t2</t>
+  </si>
+  <si>
+    <t>t3</t>
+  </si>
+  <si>
+    <t>t4</t>
+  </si>
+  <si>
+    <t>t5</t>
+  </si>
+  <si>
+    <t>t6</t>
+  </si>
+  <si>
+    <t>t7</t>
+  </si>
+  <si>
+    <t>t8</t>
+  </si>
+  <si>
+    <t>(null, IAE)</t>
+  </si>
+  <si>
+    <t>[1,2]</t>
+  </si>
+  <si>
+    <t>("",null)</t>
+  </si>
+  <si>
+    <t>[1,3,4]</t>
+  </si>
+  <si>
+    <t>TST puts</t>
+  </si>
+  <si>
+    <t>[1,3,5,6,7]</t>
+  </si>
+  <si>
+    <t>{sea}</t>
+  </si>
+  <si>
+    <t>("a","")</t>
+  </si>
+  <si>
+    <t>[1,3,5,6,8,10,6,7]</t>
+  </si>
+  <si>
+    <t>("t","")</t>
+  </si>
+  <si>
+    <t>[1,3,5,6,8,9,11,6,7]</t>
+  </si>
+  <si>
+    <t>("s","")</t>
+  </si>
+  <si>
+    <t>[1,3,5,6,8,9,12,14,6,7]</t>
+  </si>
+  <si>
+    <t>{s}</t>
+  </si>
+  <si>
+    <t>[1,3,5,6,8,9,12,13,14,6,7]</t>
+  </si>
+  <si>
+    <t>t9</t>
+  </si>
+  <si>
+    <t>t10</t>
+  </si>
+  <si>
+    <t>{s},{a}</t>
+  </si>
+  <si>
+    <t>[1,3,5,6,8,10,6,8,9,12,13,14,6,7]</t>
+  </si>
+  <si>
+    <t>{s},{u}</t>
+  </si>
+  <si>
+    <t>[1,3,5,6,8,9,11,6,8,9,12,13,14,6,7]</t>
+  </si>
+  <si>
+    <t>{sea}, {s}, {e}, {a}</t>
+  </si>
+  <si>
+    <t>[1,3,5,6,8,9,12,13,14,6,8,9,12,14,6,8,9,12,13,14,6,7]</t>
+  </si>
+  <si>
+    <t>t11</t>
+  </si>
+  <si>
+    <t>("sea","sea")</t>
+  </si>
+  <si>
+    <t>("u","u")</t>
+  </si>
+  <si>
+    <t>("a","a")</t>
+  </si>
+  <si>
+    <t>("s","s")</t>
+  </si>
+  <si>
+    <t>("set","")</t>
+  </si>
+  <si>
+    <t>[1,3,5,6,8,9,12,14,6,8,9,12,14,6,8,9,11,6,7]</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="8"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>[5,6,7]</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="9" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>[5,6,8]</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="9" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>[5,6,8,9,12]</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="9" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>[5,6,8,9,12,13]</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="9" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>[12,13]</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="9" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>[12,13,14,6,7]</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>,</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="9" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> [12,13,14,6,8]</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="9" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>[12,13,14,6,8,9,12]</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, [12,14,6,7],</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="9" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> [12,14,6,8]</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>,</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="9" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> [12,14,6,8,9,12]</t>
+    </r>
+  </si>
+  <si>
+    <t>("query","")</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="9" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>[8,9]</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>[8,10]</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>[8,9,11]</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>,</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="9" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> [8,9,12]</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>[1,2]</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="9" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>[1,3]</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="5"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>[1,3,4]</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>,</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="8"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> [1,3,5]</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="8"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>[1,3,5,6,7]</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>,</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="9" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> [1,3,5,6,8]</t>
+    </r>
+  </si>
+  <si>
+    <t>[1,3,5,6,8,10,6,8,9,11,6,8,9,12,13,14,6,7]</t>
+  </si>
+  <si>
+    <t>[1,3,5,6,8,10,6,8,10,6,8,9,12,13,14,6,7]</t>
+  </si>
+  <si>
+    <t>t12</t>
+  </si>
+  <si>
+    <t>t13</t>
+  </si>
+  <si>
+    <t>t14</t>
+  </si>
+  <si>
+    <t>[1,3,5,6,8,9,11,6,8,9,11,6,8,9,12,13,14,6,7]</t>
+  </si>
+  <si>
+    <t>[1,3,5,6,8,9,12,14,6,8,10,6,7]</t>
+  </si>
+  <si>
+    <t>[1,3,5,6,8,9,12,14,6,8,9,11,6,7]</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="9" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>[14,6,7]</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>,</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="9" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> [14,6,8]</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color rgb="FFFFC000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>[14,6,8,10]</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>,</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="9" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> [14,6,8,9]</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color rgb="FF92D050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>[14,6,8,9,11]</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>,</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="9" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> [14,6,8,9,12]</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="9" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>[14,6,8,9,12,13],</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> [14,6,8,9,12,13,14]</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="9" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, [14,6,8,9,12,14]</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="8"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>[5,6,7]</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="9"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>[5,6,8]</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>,</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> [5,6,8,10]</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>,</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="9" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> [5,6,8,9]</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="6"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>[5,6,8,9,11]</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="9" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>[5,6,8,9,12]</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="9" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>[5,6,8,9,12,13]</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="9" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>[5,6,8,9,12,13,14]</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, [5,6,8,9,12,14]</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="4" tint="0.59999389629810485"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>[10,6,7]</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>[10,6,8]</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>,</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> [10,6,8,10]</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>[10,6,8,9]</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>[10,6,8,9,11]</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>,</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> [10,6,8,9,12]</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>[10,6,8,9,12,13]</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>[10,6,8,9,12,13,14]</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, [10,6,8,9,12,14]</t>
+    </r>
+  </si>
+  <si>
+    <t>[1,3,5,6,8,9,11,6,8,10,6,7]</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="6"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>[11,6,7]</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>[11,6,8]</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color rgb="FFFF99CC"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>[11,6,8,10]</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>[11,6,8,9]</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>,</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> [11,6,8,9,11]</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>[11,6,8,9,12]</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>,</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> [11,6,8,9,12,13]</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>[11,6,8,9,12,13,14]</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, [11,6,8,9,12,14]</t>
+    </r>
+  </si>
+  <si>
+    <t>t15</t>
+  </si>
+  <si>
+    <t>t16</t>
+  </si>
+  <si>
+    <t>t17</t>
+  </si>
+  <si>
+    <t>{sea}, {t}, {a}</t>
+  </si>
+  <si>
+    <t>{sea}, {ball}, {c}</t>
+  </si>
+  <si>
+    <t>("c","c")</t>
+  </si>
+  <si>
+    <t>{sea}, {cat}, {b}</t>
+  </si>
+  <si>
+    <t>("b","b")</t>
+  </si>
+  <si>
+    <t>{sea}, {up}, {w}</t>
+  </si>
+  <si>
+    <t>("w","w")</t>
+  </si>
+  <si>
+    <t>("sd","")</t>
+  </si>
+  <si>
+    <t>{sea}, {w}</t>
+  </si>
+  <si>
+    <t>("su","")</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="31" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="5"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="9" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="9"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FF7030A0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="5"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="9" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="5" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color rgb="FF7030A0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color rgb="FFFFC000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color rgb="FF0070C0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FF0070C0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color rgb="FFC00000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FFC00000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FFFFC000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color rgb="FF92D050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FF92D050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="6"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="6"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="4" tint="0.59999389629810485"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="4" tint="0.59999389629810485"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color rgb="FFFF99CC"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FFFF99CC"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -246,7 +1752,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -260,17 +1766,71 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -278,6 +1838,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFF99CC"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -586,17 +2151,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{264CF138-5F0D-488B-AB06-FA1FA3999E91}">
-  <dimension ref="B5:H37"/>
+  <dimension ref="B5:H46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H51" sqref="H51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="4" width="18.140625" style="2" customWidth="1"/>
-    <col min="6" max="7" width="12.5703125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="89.7109375" customWidth="1"/>
+    <col min="5" max="5" width="3.42578125" customWidth="1"/>
+    <col min="6" max="7" width="16.140625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="133.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
@@ -619,12 +2185,12 @@
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="2">
         <v>1</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>11</v>
+        <v>39</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>10</v>
@@ -636,10 +2202,10 @@
         <v>1</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
         <v>12</v>
       </c>
@@ -649,8 +2215,8 @@
       <c r="D7" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
       <c r="H7" s="8"/>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
@@ -669,8 +2235,8 @@
       <c r="G8" s="4">
         <v>5</v>
       </c>
-      <c r="H8" s="7" t="s">
-        <v>38</v>
+      <c r="H8" s="9" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.25">
@@ -683,9 +2249,9 @@
       <c r="D9" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F9" s="5"/>
-      <c r="G9" s="6"/>
-      <c r="H9" s="8"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="10"/>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B10" s="2">
@@ -697,12 +2263,12 @@
       <c r="D10" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F10" s="5"/>
+      <c r="F10" s="6"/>
       <c r="G10" s="4">
         <v>13</v>
       </c>
-      <c r="H10" s="7" t="s">
-        <v>39</v>
+      <c r="H10" s="11" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
@@ -715,9 +2281,9 @@
       <c r="D11" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="F11" s="6"/>
-      <c r="G11" s="6"/>
-      <c r="H11" s="8"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="12"/>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B12" s="3" t="s">
@@ -736,7 +2302,7 @@
         <v>5</v>
       </c>
       <c r="H12" s="7" t="s">
-        <v>40</v>
+        <v>95</v>
       </c>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.25">
@@ -749,8 +2315,8 @@
       <c r="D13" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F13" s="5"/>
-      <c r="G13" s="6"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="5"/>
       <c r="H13" s="8"/>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.25">
@@ -763,12 +2329,12 @@
       <c r="D14" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="F14" s="5"/>
+      <c r="F14" s="6"/>
       <c r="G14" s="4">
         <v>10</v>
       </c>
       <c r="H14" s="7" t="s">
-        <v>42</v>
+        <v>96</v>
       </c>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.25">
@@ -781,8 +2347,8 @@
       <c r="D15" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="F15" s="5"/>
-      <c r="G15" s="6"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="5"/>
       <c r="H15" s="8"/>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
@@ -795,12 +2361,12 @@
       <c r="D16" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="F16" s="5"/>
+      <c r="F16" s="6"/>
       <c r="G16" s="4">
         <v>11</v>
       </c>
       <c r="H16" s="7" t="s">
-        <v>41</v>
+        <v>98</v>
       </c>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.25">
@@ -813,8 +2379,8 @@
       <c r="D17" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="F17" s="5"/>
-      <c r="G17" s="6"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="5"/>
       <c r="H17" s="8"/>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.25">
@@ -827,12 +2393,12 @@
       <c r="D18" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F18" s="5"/>
+      <c r="F18" s="6"/>
       <c r="G18" s="4">
         <v>14</v>
       </c>
       <c r="H18" s="7" t="s">
-        <v>43</v>
+        <v>94</v>
       </c>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.25">
@@ -845,8 +2411,8 @@
       <c r="D19" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="F19" s="6"/>
-      <c r="G19" s="6"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="5"/>
       <c r="H19" s="8"/>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.25">
@@ -866,7 +2432,7 @@
         <v>5</v>
       </c>
       <c r="H20" s="7" t="s">
-        <v>44</v>
+        <v>81</v>
       </c>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.25">
@@ -879,8 +2445,8 @@
       <c r="D21" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="F21" s="5"/>
-      <c r="G21" s="6"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="5"/>
       <c r="H21" s="8"/>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.25">
@@ -893,12 +2459,12 @@
       <c r="D22" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="F22" s="5"/>
+      <c r="F22" s="6"/>
       <c r="G22" s="4">
         <v>12</v>
       </c>
       <c r="H22" s="7" t="s">
-        <v>45</v>
+        <v>82</v>
       </c>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.25">
@@ -911,8 +2477,8 @@
       <c r="D23" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="F23" s="6"/>
-      <c r="G23" s="6"/>
+      <c r="F23" s="5"/>
+      <c r="G23" s="5"/>
       <c r="H23" s="8"/>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.25">
@@ -932,7 +2498,7 @@
         <v>8</v>
       </c>
       <c r="H24" s="7" t="s">
-        <v>46</v>
+        <v>84</v>
       </c>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.25">
@@ -945,8 +2511,8 @@
       <c r="D25" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="F25" s="6"/>
-      <c r="G25" s="6"/>
+      <c r="F25" s="5"/>
+      <c r="G25" s="5"/>
       <c r="H25" s="8"/>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.25">
@@ -968,38 +2534,275 @@
     </row>
     <row r="29" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B29" s="3"/>
-    </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="E29" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="H29" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="30" spans="2:8" ht="23.25" x14ac:dyDescent="0.25">
       <c r="B30" s="3"/>
-    </row>
-    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="E30" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G30" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="H30" s="13" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="31" spans="2:8" ht="23.25" x14ac:dyDescent="0.25">
       <c r="B31" s="3"/>
-    </row>
-    <row r="32" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="E31" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G31" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="H31" s="14" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="32" spans="2:8" ht="23.25" x14ac:dyDescent="0.25">
       <c r="B32" s="3"/>
-    </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="E32" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G32" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="H32" s="15" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="33" spans="2:8" ht="23.25" x14ac:dyDescent="0.25">
       <c r="B33" s="3"/>
-    </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="E33" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="G33" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="H33" s="25" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="34" spans="2:8" ht="23.25" x14ac:dyDescent="0.25">
       <c r="B34" s="3"/>
-    </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="E34" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="G34" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="H34" s="24" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="35" spans="2:8" ht="23.25" x14ac:dyDescent="0.25">
       <c r="B35" s="3"/>
-    </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="E35" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="G35" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="H35" s="16" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="36" spans="2:8" ht="23.25" x14ac:dyDescent="0.25">
       <c r="B36" s="3"/>
-    </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="E36" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="G36" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="H36" s="16" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="37" spans="2:8" ht="23.25" x14ac:dyDescent="0.25">
       <c r="B37" s="3"/>
+      <c r="E37" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="G37" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="H37" s="16" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="38" spans="2:8" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="E38" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="G38" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="H38" s="16" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="39" spans="2:8" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="E39" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="G39" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="H39" s="17" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="40" spans="2:8" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="E40" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="G40" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="H40" s="18" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="41" spans="2:8" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="E41" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="G41" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="H41" s="19" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="42" spans="2:8" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="E42" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="G42" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="H42" s="21" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="43" spans="2:8" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="E43" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="G43" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="H43" s="22" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="44" spans="2:8" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="E44" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="G44" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="H44" s="20" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="45" spans="2:8" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="E45" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="G45" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="H45" s="23" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="46" spans="2:8" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="E46" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="G46" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="H46" s="26" t="s">
+        <v>97</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="H6:H7"/>
-    <mergeCell ref="H8:H9"/>
-    <mergeCell ref="H10:H11"/>
-    <mergeCell ref="H12:H13"/>
-    <mergeCell ref="H14:H15"/>
+    <mergeCell ref="F8:F11"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="G18:G19"/>
+    <mergeCell ref="G20:G21"/>
+    <mergeCell ref="G22:G23"/>
+    <mergeCell ref="G6:G7"/>
+    <mergeCell ref="G8:G9"/>
+    <mergeCell ref="G10:G11"/>
     <mergeCell ref="G24:G25"/>
     <mergeCell ref="F24:F25"/>
     <mergeCell ref="F20:F23"/>
@@ -1012,15 +2815,13 @@
     <mergeCell ref="G14:G15"/>
     <mergeCell ref="G16:G17"/>
     <mergeCell ref="H16:H17"/>
-    <mergeCell ref="F8:F11"/>
-    <mergeCell ref="F6:F7"/>
-    <mergeCell ref="G18:G19"/>
-    <mergeCell ref="G20:G21"/>
-    <mergeCell ref="G22:G23"/>
-    <mergeCell ref="G6:G7"/>
-    <mergeCell ref="G8:G9"/>
-    <mergeCell ref="G10:G11"/>
+    <mergeCell ref="H6:H7"/>
+    <mergeCell ref="H8:H9"/>
+    <mergeCell ref="H10:H11"/>
+    <mergeCell ref="H12:H13"/>
+    <mergeCell ref="H14:H15"/>
   </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
removed unnecessary test for AUC
some du-path are not covered
but it's ok because we only need to satisfy AUC and not ADUPC
</commit_message>
<xml_diff>
--- a/AUC.xlsx
+++ b/AUC.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Google Drive\Faculdade\Verificação e Validação de Software\Assignment1\vvs1920_assignment1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFADDC4A-5F3C-4D96-81E2-5BC10EF7BD90}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F9E7294-093F-4C4B-8FA2-01C7E6C0E03A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-7455" yWindow="5910" windowWidth="15375" windowHeight="7965" xr2:uid="{E18B8583-D319-4337-B06E-00832F8818CE}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="97">
   <si>
     <t>query</t>
   </si>
@@ -221,36 +221,12 @@
     <t>[1,3,5,6,8,9,11,6,7]</t>
   </si>
   <si>
-    <t>("s","")</t>
-  </si>
-  <si>
-    <t>[1,3,5,6,8,9,12,14,6,7]</t>
-  </si>
-  <si>
-    <t>{s}</t>
-  </si>
-  <si>
-    <t>[1,3,5,6,8,9,12,13,14,6,7]</t>
-  </si>
-  <si>
     <t>t9</t>
   </si>
   <si>
     <t>t10</t>
   </si>
   <si>
-    <t>{s},{a}</t>
-  </si>
-  <si>
-    <t>[1,3,5,6,8,10,6,8,9,12,13,14,6,7]</t>
-  </si>
-  <si>
-    <t>{s},{u}</t>
-  </si>
-  <si>
-    <t>[1,3,5,6,8,9,11,6,8,9,12,13,14,6,7]</t>
-  </si>
-  <si>
     <t>{sea}, {s}, {e}, {a}</t>
   </si>
   <si>
@@ -263,15 +239,6 @@
     <t>("sea","sea")</t>
   </si>
   <si>
-    <t>("u","u")</t>
-  </si>
-  <si>
-    <t>("a","a")</t>
-  </si>
-  <si>
-    <t>("s","s")</t>
-  </si>
-  <si>
     <t>("set","")</t>
   </si>
   <si>
@@ -697,9 +664,6 @@
     <t>t13</t>
   </si>
   <si>
-    <t>t14</t>
-  </si>
-  <si>
     <t>[1,3,5,6,8,9,11,6,8,9,11,6,8,9,12,13,14,6,7]</t>
   </si>
   <si>
@@ -1404,15 +1368,6 @@
       </rPr>
       <t>, [11,6,8,9,12,14]</t>
     </r>
-  </si>
-  <si>
-    <t>t15</t>
-  </si>
-  <si>
-    <t>t16</t>
-  </si>
-  <si>
-    <t>t17</t>
   </si>
   <si>
     <t>{sea}, {t}, {a}</t>
@@ -1449,7 +1404,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="31" x14ac:knownFonts="1">
+  <fonts count="30" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1546,14 +1501,6 @@
       <b/>
       <sz val="18"/>
       <color theme="8"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1752,7 +1699,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1762,33 +1709,6 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1814,23 +1734,47 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2151,10 +2095,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{264CF138-5F0D-488B-AB06-FA1FA3999E91}">
-  <dimension ref="B5:H46"/>
+  <dimension ref="B5:H42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H51" sqref="H51"/>
+    <sheetView tabSelected="1" topLeftCell="E10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H47" sqref="H47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2195,14 +2139,14 @@
       <c r="D6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="F6" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="G6" s="4">
+      <c r="G6" s="17">
         <v>1</v>
       </c>
-      <c r="H6" s="7" t="s">
-        <v>85</v>
+      <c r="H6" s="20" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="7" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2215,9 +2159,9 @@
       <c r="D7" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="8"/>
+      <c r="F7" s="19"/>
+      <c r="G7" s="19"/>
+      <c r="H7" s="21"/>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B8" s="2">
@@ -2229,13 +2173,13 @@
       <c r="D8" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F8" s="4" t="s">
+      <c r="F8" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="G8" s="4">
+      <c r="G8" s="17">
         <v>5</v>
       </c>
-      <c r="H8" s="9" t="s">
+      <c r="H8" s="22" t="s">
         <v>37</v>
       </c>
     </row>
@@ -2249,9 +2193,9 @@
       <c r="D9" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F9" s="6"/>
-      <c r="G9" s="5"/>
-      <c r="H9" s="10"/>
+      <c r="F9" s="18"/>
+      <c r="G9" s="19"/>
+      <c r="H9" s="23"/>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B10" s="2">
@@ -2263,11 +2207,11 @@
       <c r="D10" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F10" s="6"/>
-      <c r="G10" s="4">
+      <c r="F10" s="18"/>
+      <c r="G10" s="17">
         <v>13</v>
       </c>
-      <c r="H10" s="11" t="s">
+      <c r="H10" s="24" t="s">
         <v>38</v>
       </c>
     </row>
@@ -2281,9 +2225,9 @@
       <c r="D11" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="F11" s="5"/>
-      <c r="G11" s="5"/>
-      <c r="H11" s="12"/>
+      <c r="F11" s="19"/>
+      <c r="G11" s="19"/>
+      <c r="H11" s="25"/>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B12" s="3" t="s">
@@ -2295,14 +2239,14 @@
       <c r="D12" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F12" s="4" t="s">
+      <c r="F12" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="G12" s="4">
+      <c r="G12" s="17">
         <v>5</v>
       </c>
-      <c r="H12" s="7" t="s">
-        <v>95</v>
+      <c r="H12" s="20" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.25">
@@ -2315,9 +2259,9 @@
       <c r="D13" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F13" s="6"/>
-      <c r="G13" s="5"/>
-      <c r="H13" s="8"/>
+      <c r="F13" s="18"/>
+      <c r="G13" s="19"/>
+      <c r="H13" s="21"/>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B14" s="3" t="s">
@@ -2329,12 +2273,12 @@
       <c r="D14" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="F14" s="6"/>
-      <c r="G14" s="4">
+      <c r="F14" s="18"/>
+      <c r="G14" s="17">
         <v>10</v>
       </c>
-      <c r="H14" s="7" t="s">
-        <v>96</v>
+      <c r="H14" s="20" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.25">
@@ -2347,9 +2291,9 @@
       <c r="D15" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="F15" s="6"/>
-      <c r="G15" s="5"/>
-      <c r="H15" s="8"/>
+      <c r="F15" s="18"/>
+      <c r="G15" s="19"/>
+      <c r="H15" s="21"/>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B16" s="2">
@@ -2361,12 +2305,12 @@
       <c r="D16" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="F16" s="6"/>
-      <c r="G16" s="4">
+      <c r="F16" s="18"/>
+      <c r="G16" s="17">
         <v>11</v>
       </c>
-      <c r="H16" s="7" t="s">
-        <v>98</v>
+      <c r="H16" s="20" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.25">
@@ -2379,9 +2323,9 @@
       <c r="D17" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="F17" s="6"/>
-      <c r="G17" s="5"/>
-      <c r="H17" s="8"/>
+      <c r="F17" s="18"/>
+      <c r="G17" s="19"/>
+      <c r="H17" s="21"/>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B18" s="3" t="s">
@@ -2393,12 +2337,12 @@
       <c r="D18" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F18" s="6"/>
-      <c r="G18" s="4">
+      <c r="F18" s="18"/>
+      <c r="G18" s="17">
         <v>14</v>
       </c>
-      <c r="H18" s="7" t="s">
-        <v>94</v>
+      <c r="H18" s="20" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.25">
@@ -2411,9 +2355,9 @@
       <c r="D19" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="F19" s="5"/>
-      <c r="G19" s="5"/>
-      <c r="H19" s="8"/>
+      <c r="F19" s="19"/>
+      <c r="G19" s="19"/>
+      <c r="H19" s="21"/>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B20" s="3" t="s">
@@ -2425,14 +2369,14 @@
       <c r="D20" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F20" s="4" t="s">
+      <c r="F20" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="G20" s="4">
+      <c r="G20" s="17">
         <v>5</v>
       </c>
-      <c r="H20" s="7" t="s">
-        <v>81</v>
+      <c r="H20" s="20" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.25">
@@ -2445,9 +2389,9 @@
       <c r="D21" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="F21" s="6"/>
-      <c r="G21" s="5"/>
-      <c r="H21" s="8"/>
+      <c r="F21" s="18"/>
+      <c r="G21" s="19"/>
+      <c r="H21" s="21"/>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B22" s="3" t="s">
@@ -2459,12 +2403,12 @@
       <c r="D22" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="F22" s="6"/>
-      <c r="G22" s="4">
+      <c r="F22" s="18"/>
+      <c r="G22" s="17">
         <v>12</v>
       </c>
-      <c r="H22" s="7" t="s">
-        <v>82</v>
+      <c r="H22" s="20" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.25">
@@ -2477,9 +2421,9 @@
       <c r="D23" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="F23" s="5"/>
-      <c r="G23" s="5"/>
-      <c r="H23" s="8"/>
+      <c r="F23" s="19"/>
+      <c r="G23" s="19"/>
+      <c r="H23" s="21"/>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B24" s="3" t="s">
@@ -2491,14 +2435,14 @@
       <c r="D24" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="F24" s="4" t="s">
+      <c r="F24" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="G24" s="4">
+      <c r="G24" s="17">
         <v>8</v>
       </c>
-      <c r="H24" s="7" t="s">
-        <v>84</v>
+      <c r="H24" s="20" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.25">
@@ -2511,9 +2455,9 @@
       <c r="D25" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="F25" s="5"/>
-      <c r="G25" s="5"/>
-      <c r="H25" s="8"/>
+      <c r="F25" s="19"/>
+      <c r="G25" s="19"/>
+      <c r="H25" s="21"/>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B26" s="3" t="s">
@@ -2558,7 +2502,7 @@
       <c r="G30" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="H30" s="13" t="s">
+      <c r="H30" s="4" t="s">
         <v>52</v>
       </c>
     </row>
@@ -2573,7 +2517,7 @@
       <c r="G31" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="H31" s="14" t="s">
+      <c r="H31" s="5" t="s">
         <v>54</v>
       </c>
     </row>
@@ -2586,9 +2530,9 @@
         <v>10</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="H32" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="H32" s="6" t="s">
         <v>56</v>
       </c>
     </row>
@@ -2603,7 +2547,7 @@
       <c r="G33" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="H33" s="25" t="s">
+      <c r="H33" s="15" t="s">
         <v>59</v>
       </c>
     </row>
@@ -2618,7 +2562,7 @@
       <c r="G34" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="H34" s="24" t="s">
+      <c r="H34" s="14" t="s">
         <v>61</v>
       </c>
     </row>
@@ -2628,13 +2572,13 @@
         <v>48</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="H35" s="16" t="s">
-        <v>63</v>
+        <v>67</v>
+      </c>
+      <c r="H35" s="7" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="36" spans="2:8" ht="23.25" x14ac:dyDescent="0.25">
@@ -2643,13 +2587,13 @@
         <v>49</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>64</v>
+        <v>87</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="H36" s="16" t="s">
-        <v>65</v>
+        <v>68</v>
+      </c>
+      <c r="H36" s="8" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="37" spans="2:8" ht="23.25" x14ac:dyDescent="0.25">
@@ -2658,151 +2602,92 @@
         <v>50</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="G37" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="H37" s="16" t="s">
-        <v>69</v>
+        <v>88</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="H37" s="9" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="38" spans="2:8" ht="23.25" x14ac:dyDescent="0.25">
       <c r="E38" s="2" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="G38" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="G38" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="H38" s="11" t="s">
         <v>76</v>
-      </c>
-      <c r="H38" s="16" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="39" spans="2:8" ht="23.25" x14ac:dyDescent="0.25">
       <c r="E39" s="2" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="G39" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="H39" s="17" t="s">
-        <v>73</v>
+        <v>92</v>
+      </c>
+      <c r="G39" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="H39" s="12" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="40" spans="2:8" ht="23.25" x14ac:dyDescent="0.25">
       <c r="E40" s="2" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="G40" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="H40" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="G40" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="H40" s="10" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="41" spans="2:8" ht="23.25" x14ac:dyDescent="0.25">
       <c r="E41" s="2" t="s">
-        <v>88</v>
+        <v>77</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>103</v>
+        <v>57</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="H41" s="19" t="s">
-        <v>86</v>
+        <v>96</v>
+      </c>
+      <c r="H41" s="13" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="42" spans="2:8" ht="23.25" x14ac:dyDescent="0.25">
       <c r="E42" s="2" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="H42" s="21" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="43" spans="2:8" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="E43" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="F43" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="G43" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="H43" s="22" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="44" spans="2:8" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="E44" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="F44" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="G44" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="H44" s="20" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="45" spans="2:8" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="E45" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="F45" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="G45" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="H45" s="23" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="46" spans="2:8" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="E46" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="F46" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="G46" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="H46" s="26" t="s">
-        <v>97</v>
+      <c r="H42" s="16" t="s">
+        <v>85</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="F8:F11"/>
-    <mergeCell ref="F6:F7"/>
-    <mergeCell ref="G18:G19"/>
-    <mergeCell ref="G20:G21"/>
-    <mergeCell ref="G22:G23"/>
-    <mergeCell ref="G6:G7"/>
-    <mergeCell ref="G8:G9"/>
-    <mergeCell ref="G10:G11"/>
+    <mergeCell ref="H6:H7"/>
+    <mergeCell ref="H8:H9"/>
+    <mergeCell ref="H10:H11"/>
+    <mergeCell ref="H12:H13"/>
+    <mergeCell ref="H14:H15"/>
     <mergeCell ref="G24:G25"/>
     <mergeCell ref="F24:F25"/>
     <mergeCell ref="F20:F23"/>
@@ -2815,11 +2700,14 @@
     <mergeCell ref="G14:G15"/>
     <mergeCell ref="G16:G17"/>
     <mergeCell ref="H16:H17"/>
-    <mergeCell ref="H6:H7"/>
-    <mergeCell ref="H8:H9"/>
-    <mergeCell ref="H10:H11"/>
-    <mergeCell ref="H12:H13"/>
-    <mergeCell ref="H14:H15"/>
+    <mergeCell ref="F8:F11"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="G18:G19"/>
+    <mergeCell ref="G20:G21"/>
+    <mergeCell ref="G22:G23"/>
+    <mergeCell ref="G6:G7"/>
+    <mergeCell ref="G8:G9"/>
+    <mergeCell ref="G10:G11"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added AUC test set table, minor docs update
</commit_message>
<xml_diff>
--- a/AUC.xlsx
+++ b/AUC.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Google Drive\Faculdade\Verificação e Validação de Software\Assignment1\vvs1920_assignment1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A34F0C82-BCCD-4CCD-8122-8AE9B850F949}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A47C5A66-041B-4A3B-B60A-7A2B372D03DD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E18B8583-D319-4337-B06E-00832F8818CE}"/>
+    <workbookView xWindow="21090" yWindow="4770" windowWidth="15375" windowHeight="7965" xr2:uid="{E18B8583-D319-4337-B06E-00832F8818CE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -677,6 +677,546 @@
       <rPr>
         <b/>
         <sz val="14"/>
+        <color theme="4" tint="0.59999389629810485"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>[10,6,7]</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>[10,6,8]</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>,</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> [10,6,8,10]</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>[10,6,8,9]</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>[10,6,8,9,11]</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>,</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> [10,6,8,9,12]</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>[10,6,8,9,12,13]</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>[10,6,8,9,12,13,14]</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, [10,6,8,9,12,14]</t>
+    </r>
+  </si>
+  <si>
+    <t>[1,3,5,6,8,9,11,6,8,10,6,7]</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="6"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>[11,6,7]</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>[11,6,8]</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color rgb="FFFF99CC"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>[11,6,8,10]</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>[11,6,8,9]</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>,</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> [11,6,8,9,11]</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>[11,6,8,9,12]</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>,</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> [11,6,8,9,12,13]</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>[11,6,8,9,12,13,14]</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, [11,6,8,9,12,14]</t>
+    </r>
+  </si>
+  <si>
+    <t>{sea}, {t}, {a}</t>
+  </si>
+  <si>
+    <t>{sea}, {ball}, {c}</t>
+  </si>
+  <si>
+    <t>("c","c")</t>
+  </si>
+  <si>
+    <t>{sea}, {cat}, {b}</t>
+  </si>
+  <si>
+    <t>("b","b")</t>
+  </si>
+  <si>
+    <t>{sea}, {up}, {w}</t>
+  </si>
+  <si>
+    <t>("w","w")</t>
+  </si>
+  <si>
+    <t>("sd","")</t>
+  </si>
+  <si>
+    <t>{sea}, {w}</t>
+  </si>
+  <si>
+    <t>("su","")</t>
+  </si>
+  <si>
+    <t>root</t>
+  </si>
+  <si>
+    <t>[1,3,5]</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="9" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>[14,6,7]</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>,</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="9" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> [14,6,8]</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color rgb="FFFFC000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>[14,6,8,10]</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>,</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="9" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> [14,6,8,9]</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color rgb="FF92D050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>[14,6,8,9,11]</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>,</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="9" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> [14,6,8,9,12]</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="9" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>[14,6,8,9,12,13], [14,6,8,9,12,13,14], [14,6,8,9,12,14]</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
         <color theme="8"/>
         <rFont val="Calibri"/>
         <family val="2"/>
@@ -840,547 +1380,18 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>, [5,6,8,9,12,14]</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color theme="4" tint="0.59999389629810485"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>[10,6,7]</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">, </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color rgb="FF7030A0"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>[10,6,8]</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>,</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> [10,6,8,10]</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">, </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color rgb="FF7030A0"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>[10,6,8,9]</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">, </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color rgb="FF7030A0"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>[10,6,8,9,11]</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>,</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> [10,6,8,9,12]</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">, </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>[10,6,8,9,12,13]</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">, </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>[10,6,8,9,12,13,14]</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>, [10,6,8,9,12,14]</t>
-    </r>
-  </si>
-  <si>
-    <t>[1,3,5,6,8,9,11,6,8,10,6,7]</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color theme="6"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>[11,6,7]</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">, </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color rgb="FF7030A0"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>[11,6,8]</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">, </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color rgb="FFFF99CC"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>[11,6,8,10]</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">, </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color rgb="FFC00000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>[11,6,8,9]</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>,</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color rgb="FFC00000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> [11,6,8,9,11]</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">, </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color rgb="FF7030A0"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>[11,6,8,9,12]</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>,</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color rgb="FFC00000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> [11,6,8,9,12,13]</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">, </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color rgb="FFC00000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>[11,6,8,9,12,13,14]</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>, [11,6,8,9,12,14]</t>
-    </r>
-  </si>
-  <si>
-    <t>{sea}, {t}, {a}</t>
-  </si>
-  <si>
-    <t>{sea}, {ball}, {c}</t>
-  </si>
-  <si>
-    <t>("c","c")</t>
-  </si>
-  <si>
-    <t>{sea}, {cat}, {b}</t>
-  </si>
-  <si>
-    <t>("b","b")</t>
-  </si>
-  <si>
-    <t>{sea}, {up}, {w}</t>
-  </si>
-  <si>
-    <t>("w","w")</t>
-  </si>
-  <si>
-    <t>("sd","")</t>
-  </si>
-  <si>
-    <t>{sea}, {w}</t>
-  </si>
-  <si>
-    <t>("su","")</t>
-  </si>
-  <si>
-    <t>root</t>
-  </si>
-  <si>
-    <t>[1,3,5]</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color theme="9" tint="-0.249977111117893"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>[14,6,7]</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>,</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color theme="9" tint="-0.249977111117893"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> [14,6,8]</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">, </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color rgb="FFFFC000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>[14,6,8,10]</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>,</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color theme="9" tint="-0.249977111117893"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> [14,6,8,9]</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">, </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color rgb="FF92D050"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>[14,6,8,9,11]</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>,</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color theme="9" tint="-0.249977111117893"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> [14,6,8,9,12]</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">, </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color theme="9" tint="-0.249977111117893"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>[14,6,8,9,12,13], [14,6,8,9,12,13,14], [14,6,8,9,12,14]</t>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="5" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>[5,6,8,9,12,14]</t>
     </r>
   </si>
 </sst>
@@ -1388,7 +1399,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="31" x14ac:knownFonts="1">
+  <fonts count="32" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1628,6 +1639,14 @@
     <font>
       <sz val="14"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="5" tint="-0.249977111117893"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1740,6 +1759,21 @@
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1757,21 +1791,6 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -2097,8 +2116,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{264CF138-5F0D-488B-AB06-FA1FA3999E91}">
   <dimension ref="B3:H42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H42" sqref="H42"/>
+    <sheetView tabSelected="1" topLeftCell="G7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12:H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2122,368 +2141,368 @@
       </c>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="F4" s="23" t="s">
+      <c r="F4" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="G4" s="23">
+      <c r="G4" s="19">
         <v>1</v>
       </c>
-      <c r="H4" s="17" t="s">
+      <c r="H4" s="22" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="5" spans="2:8" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B5" s="26" t="s">
+      <c r="B5" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="26" t="s">
+      <c r="C5" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="26" t="s">
+      <c r="D5" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="F5" s="24"/>
-      <c r="G5" s="24"/>
-      <c r="H5" s="18"/>
+      <c r="F5" s="21"/>
+      <c r="G5" s="21"/>
+      <c r="H5" s="23"/>
     </row>
     <row r="6" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="26">
+      <c r="B6" s="17">
         <v>1</v>
       </c>
-      <c r="C6" s="26" t="s">
+      <c r="C6" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="D6" s="26" t="s">
+      <c r="D6" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="F6" s="23" t="s">
+      <c r="F6" s="19" t="s">
+        <v>95</v>
+      </c>
+      <c r="G6" s="19">
+        <v>1</v>
+      </c>
+      <c r="H6" s="24" t="s">
         <v>96</v>
       </c>
-      <c r="G6" s="23">
+    </row>
+    <row r="7" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" s="21"/>
+      <c r="G7" s="21"/>
+      <c r="H7" s="28"/>
+    </row>
+    <row r="8" spans="2:8" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="B8" s="17">
+        <v>3</v>
+      </c>
+      <c r="C8" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="F8" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="H6" s="19" t="s">
+      <c r="G8" s="19">
+        <v>5</v>
+      </c>
+      <c r="H8" s="24" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="B9" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="F9" s="20"/>
+      <c r="G9" s="21"/>
+      <c r="H9" s="25"/>
+    </row>
+    <row r="10" spans="2:8" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="B10" s="17">
+        <v>4</v>
+      </c>
+      <c r="C10" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="F10" s="20"/>
+      <c r="G10" s="19">
+        <v>13</v>
+      </c>
+      <c r="H10" s="26" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="B11" s="17">
+        <v>5</v>
+      </c>
+      <c r="C11" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="F11" s="21"/>
+      <c r="G11" s="21"/>
+      <c r="H11" s="27"/>
+    </row>
+    <row r="12" spans="2:8" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="B12" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="F12" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="G12" s="19">
+        <v>5</v>
+      </c>
+      <c r="H12" s="22" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="B13" s="17">
+        <v>6</v>
+      </c>
+      <c r="C13" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="F13" s="20"/>
+      <c r="G13" s="21"/>
+      <c r="H13" s="23"/>
+    </row>
+    <row r="14" spans="2:8" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="B14" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="D14" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="F14" s="20"/>
+      <c r="G14" s="19">
+        <v>10</v>
+      </c>
+      <c r="H14" s="22" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="B15" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="C15" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="D15" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="F15" s="20"/>
+      <c r="G15" s="21"/>
+      <c r="H15" s="23"/>
+    </row>
+    <row r="16" spans="2:8" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="B16" s="17">
+        <v>8</v>
+      </c>
+      <c r="C16" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="D16" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="F16" s="20"/>
+      <c r="G16" s="19">
+        <v>11</v>
+      </c>
+      <c r="H16" s="22" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="B17" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="C17" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="D17" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="F17" s="20"/>
+      <c r="G17" s="21"/>
+      <c r="H17" s="23"/>
+    </row>
+    <row r="18" spans="2:8" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="B18" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="C18" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="D18" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="F18" s="20"/>
+      <c r="G18" s="19">
+        <v>14</v>
+      </c>
+      <c r="H18" s="22" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="7" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="26" t="s">
+    <row r="19" spans="2:8" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="B19" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="C19" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="D19" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="F19" s="21"/>
+      <c r="G19" s="21"/>
+      <c r="H19" s="23"/>
+    </row>
+    <row r="20" spans="2:8" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="B20" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="C20" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="D20" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="F20" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="G20" s="19">
+        <v>5</v>
+      </c>
+      <c r="H20" s="22" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="B21" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="C21" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="D21" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="F21" s="20"/>
+      <c r="G21" s="21"/>
+      <c r="H21" s="23"/>
+    </row>
+    <row r="22" spans="2:8" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="B22" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="C22" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="D22" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="F22" s="20"/>
+      <c r="G22" s="19">
         <v>12</v>
       </c>
-      <c r="C7" s="26" t="s">
+      <c r="H22" s="22" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="B23" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="C23" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="D23" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="F23" s="21"/>
+      <c r="G23" s="21"/>
+      <c r="H23" s="23"/>
+    </row>
+    <row r="24" spans="2:8" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="B24" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="C24" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="26" t="s">
-        <v>11</v>
-      </c>
-      <c r="F7" s="24"/>
-      <c r="G7" s="24"/>
-      <c r="H7" s="28"/>
-    </row>
-    <row r="8" spans="2:8" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B8" s="26">
-        <v>3</v>
-      </c>
-      <c r="C8" s="26" t="s">
-        <v>10</v>
-      </c>
-      <c r="D8" s="26" t="s">
-        <v>10</v>
-      </c>
-      <c r="F8" s="23" t="s">
-        <v>1</v>
-      </c>
-      <c r="G8" s="23">
-        <v>5</v>
-      </c>
-      <c r="H8" s="19" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="9" spans="2:8" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B9" s="26" t="s">
-        <v>13</v>
-      </c>
-      <c r="C9" s="26" t="s">
-        <v>10</v>
-      </c>
-      <c r="D9" s="26" t="s">
-        <v>11</v>
-      </c>
-      <c r="F9" s="25"/>
-      <c r="G9" s="24"/>
-      <c r="H9" s="20"/>
-    </row>
-    <row r="10" spans="2:8" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B10" s="26">
+      <c r="D24" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="F24" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="C10" s="26" t="s">
-        <v>10</v>
-      </c>
-      <c r="D10" s="26" t="s">
-        <v>10</v>
-      </c>
-      <c r="F10" s="25"/>
-      <c r="G10" s="23">
-        <v>13</v>
-      </c>
-      <c r="H10" s="21" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="11" spans="2:8" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B11" s="26">
-        <v>5</v>
-      </c>
-      <c r="C11" s="26" t="s">
-        <v>28</v>
-      </c>
-      <c r="D11" s="26" t="s">
-        <v>27</v>
-      </c>
-      <c r="F11" s="24"/>
-      <c r="G11" s="24"/>
-      <c r="H11" s="22"/>
-    </row>
-    <row r="12" spans="2:8" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B12" s="27" t="s">
-        <v>14</v>
-      </c>
-      <c r="C12" s="26" t="s">
-        <v>10</v>
-      </c>
-      <c r="D12" s="26" t="s">
-        <v>10</v>
-      </c>
-      <c r="F12" s="23" t="s">
-        <v>2</v>
-      </c>
-      <c r="G12" s="23">
-        <v>5</v>
-      </c>
-      <c r="H12" s="17" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="13" spans="2:8" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B13" s="26">
-        <v>6</v>
-      </c>
-      <c r="C13" s="26" t="s">
-        <v>10</v>
-      </c>
-      <c r="D13" s="26" t="s">
-        <v>10</v>
-      </c>
-      <c r="F13" s="25"/>
-      <c r="G13" s="24"/>
-      <c r="H13" s="18"/>
-    </row>
-    <row r="14" spans="2:8" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B14" s="27" t="s">
-        <v>15</v>
-      </c>
-      <c r="C14" s="26" t="s">
-        <v>10</v>
-      </c>
-      <c r="D14" s="26" t="s">
-        <v>29</v>
-      </c>
-      <c r="F14" s="25"/>
-      <c r="G14" s="23">
-        <v>10</v>
-      </c>
-      <c r="H14" s="17" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="15" spans="2:8" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B15" s="27" t="s">
-        <v>16</v>
-      </c>
-      <c r="C15" s="26" t="s">
-        <v>10</v>
-      </c>
-      <c r="D15" s="26" t="s">
-        <v>30</v>
-      </c>
-      <c r="F15" s="25"/>
-      <c r="G15" s="24"/>
-      <c r="H15" s="18"/>
-    </row>
-    <row r="16" spans="2:8" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B16" s="26">
+      <c r="G24" s="19">
         <v>8</v>
       </c>
-      <c r="C16" s="26" t="s">
-        <v>31</v>
-      </c>
-      <c r="D16" s="26" t="s">
+      <c r="H24" s="22" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="B25" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="C25" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="D25" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="F16" s="25"/>
-      <c r="G16" s="23">
-        <v>11</v>
-      </c>
-      <c r="H16" s="17" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="17" spans="2:8" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B17" s="27" t="s">
-        <v>17</v>
-      </c>
-      <c r="C17" s="26" t="s">
-        <v>10</v>
-      </c>
-      <c r="D17" s="26" t="s">
-        <v>33</v>
-      </c>
-      <c r="F17" s="25"/>
-      <c r="G17" s="24"/>
-      <c r="H17" s="18"/>
-    </row>
-    <row r="18" spans="2:8" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B18" s="27" t="s">
-        <v>18</v>
-      </c>
-      <c r="C18" s="26" t="s">
-        <v>10</v>
-      </c>
-      <c r="D18" s="26" t="s">
-        <v>10</v>
-      </c>
-      <c r="F18" s="25"/>
-      <c r="G18" s="23">
-        <v>14</v>
-      </c>
-      <c r="H18" s="17" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="19" spans="2:8" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B19" s="27" t="s">
-        <v>19</v>
-      </c>
-      <c r="C19" s="26" t="s">
+      <c r="F25" s="21"/>
+      <c r="G25" s="21"/>
+      <c r="H25" s="23"/>
+    </row>
+    <row r="26" spans="2:8" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="B26" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="C26" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="D19" s="26" t="s">
-        <v>34</v>
-      </c>
-      <c r="F19" s="24"/>
-      <c r="G19" s="24"/>
-      <c r="H19" s="18"/>
-    </row>
-    <row r="20" spans="2:8" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B20" s="27" t="s">
-        <v>22</v>
-      </c>
-      <c r="C20" s="26" t="s">
-        <v>10</v>
-      </c>
-      <c r="D20" s="26" t="s">
-        <v>10</v>
-      </c>
-      <c r="F20" s="23" t="s">
-        <v>3</v>
-      </c>
-      <c r="G20" s="23">
-        <v>5</v>
-      </c>
-      <c r="H20" s="17" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="21" spans="2:8" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B21" s="26" t="s">
-        <v>23</v>
-      </c>
-      <c r="C21" s="26" t="s">
-        <v>10</v>
-      </c>
-      <c r="D21" s="26" t="s">
-        <v>33</v>
-      </c>
-      <c r="F21" s="25"/>
-      <c r="G21" s="24"/>
-      <c r="H21" s="18"/>
-    </row>
-    <row r="22" spans="2:8" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B22" s="27" t="s">
-        <v>20</v>
-      </c>
-      <c r="C22" s="26" t="s">
-        <v>34</v>
-      </c>
-      <c r="D22" s="26" t="s">
-        <v>34</v>
-      </c>
-      <c r="F22" s="25"/>
-      <c r="G22" s="23">
-        <v>12</v>
-      </c>
-      <c r="H22" s="17" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="23" spans="2:8" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B23" s="27" t="s">
-        <v>21</v>
-      </c>
-      <c r="C23" s="26" t="s">
-        <v>32</v>
-      </c>
-      <c r="D23" s="26" t="s">
-        <v>32</v>
-      </c>
-      <c r="F23" s="24"/>
-      <c r="G23" s="24"/>
-      <c r="H23" s="18"/>
-    </row>
-    <row r="24" spans="2:8" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B24" s="27" t="s">
-        <v>24</v>
-      </c>
-      <c r="C24" s="26" t="s">
-        <v>10</v>
-      </c>
-      <c r="D24" s="26" t="s">
-        <v>34</v>
-      </c>
-      <c r="F24" s="23" t="s">
-        <v>4</v>
-      </c>
-      <c r="G24" s="23">
-        <v>8</v>
-      </c>
-      <c r="H24" s="17" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="25" spans="2:8" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B25" s="27" t="s">
-        <v>25</v>
-      </c>
-      <c r="C25" s="26" t="s">
-        <v>35</v>
-      </c>
-      <c r="D25" s="26" t="s">
-        <v>32</v>
-      </c>
-      <c r="F25" s="24"/>
-      <c r="G25" s="24"/>
-      <c r="H25" s="18"/>
-    </row>
-    <row r="26" spans="2:8" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B26" s="27" t="s">
-        <v>26</v>
-      </c>
-      <c r="C26" s="26" t="s">
-        <v>34</v>
-      </c>
-      <c r="D26" s="26" t="s">
+      <c r="D26" s="17" t="s">
         <v>34</v>
       </c>
     </row>
@@ -2604,7 +2623,7 @@
         <v>49</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G36" s="2" t="s">
         <v>68</v>
@@ -2619,10 +2638,10 @@
         <v>50</v>
       </c>
       <c r="F37" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="G37" s="1" t="s">
         <v>87</v>
-      </c>
-      <c r="G37" s="1" t="s">
-        <v>88</v>
       </c>
       <c r="H37" s="9" t="s">
         <v>75</v>
@@ -2633,10 +2652,10 @@
         <v>62</v>
       </c>
       <c r="F38" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="G38" s="1" t="s">
         <v>89</v>
-      </c>
-      <c r="G38" s="1" t="s">
-        <v>90</v>
       </c>
       <c r="H38" s="11" t="s">
         <v>76</v>
@@ -2647,10 +2666,10 @@
         <v>63</v>
       </c>
       <c r="F39" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="G39" s="1" t="s">
         <v>91</v>
-      </c>
-      <c r="G39" s="1" t="s">
-        <v>92</v>
       </c>
       <c r="H39" s="12" t="s">
         <v>79</v>
@@ -2664,7 +2683,7 @@
         <v>57</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H40" s="10" t="s">
         <v>80</v>
@@ -2678,7 +2697,7 @@
         <v>57</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H41" s="13" t="s">
         <v>81</v>
@@ -2689,27 +2708,23 @@
         <v>78</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G42" s="1" t="s">
         <v>60</v>
       </c>
       <c r="H42" s="16" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="F8:F11"/>
-    <mergeCell ref="F4:F5"/>
-    <mergeCell ref="G18:G19"/>
-    <mergeCell ref="G20:G21"/>
-    <mergeCell ref="G22:G23"/>
-    <mergeCell ref="G4:G5"/>
-    <mergeCell ref="G8:G9"/>
-    <mergeCell ref="G10:G11"/>
-    <mergeCell ref="F6:F7"/>
-    <mergeCell ref="G6:G7"/>
+    <mergeCell ref="H4:H5"/>
+    <mergeCell ref="H8:H9"/>
+    <mergeCell ref="H10:H11"/>
+    <mergeCell ref="H12:H13"/>
+    <mergeCell ref="H14:H15"/>
+    <mergeCell ref="H6:H7"/>
     <mergeCell ref="G24:G25"/>
     <mergeCell ref="F24:F25"/>
     <mergeCell ref="F20:F23"/>
@@ -2722,12 +2737,16 @@
     <mergeCell ref="G14:G15"/>
     <mergeCell ref="G16:G17"/>
     <mergeCell ref="H16:H17"/>
-    <mergeCell ref="H4:H5"/>
-    <mergeCell ref="H8:H9"/>
-    <mergeCell ref="H10:H11"/>
-    <mergeCell ref="H12:H13"/>
-    <mergeCell ref="H14:H15"/>
-    <mergeCell ref="H6:H7"/>
+    <mergeCell ref="F8:F11"/>
+    <mergeCell ref="F4:F5"/>
+    <mergeCell ref="G18:G19"/>
+    <mergeCell ref="G20:G21"/>
+    <mergeCell ref="G22:G23"/>
+    <mergeCell ref="G4:G5"/>
+    <mergeCell ref="G8:G9"/>
+    <mergeCell ref="G10:G11"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="G6:G7"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>